<commit_message>
ostatni commit niedziela 01.09.2019
</commit_message>
<xml_diff>
--- a/TODO_lic.xlsx
+++ b/TODO_lic.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="81">
   <si>
     <t>Zadanie</t>
   </si>
@@ -187,7 +187,7 @@
     <t>Połączyć dwa rozdziały w jeden</t>
   </si>
   <si>
-    <t>rozszerzyć podrozdział i dać przykłady obliczania p-stw modelu błędu</t>
+    <t>rozszerzyć podrozdział i dać przykłady obliczania p-stw modelu błędu (na podstawie powalający)</t>
   </si>
   <si>
     <t>dopisać wzór na accuracy</t>
@@ -214,9 +214,6 @@
     <t>Zaznaczyć kolorami transformację kandydatów na błąd (jak w rozdziale 4.2)</t>
   </si>
   <si>
-    <t>Który model poradził sobie najlepiej, w której kategorii (od ogólnego podziału na trzykategoriowy podział)</t>
-  </si>
-  <si>
     <t>Analiza odpowiedzi dla test set: sprawdzić dla której lambdy mam najwyższą skuteczność w bigram_case</t>
   </si>
   <si>
@@ -247,7 +244,7 @@
     <t>tabelka z odpowiedziami dla różnych modeli - dwie sytuacje: unigram daje dobrą, inne złą oraz unigram daje złą inne dobrą - rodzaj operacji</t>
   </si>
   <si>
-    <t>Napisać, że noisy channle model nie zwraca w przypadku bigramu dla dwóch obserwacji, bo nie ma błędu w zdaniu.</t>
+    <t>Napisać, że noisy channle model nie zwraca w przypadku bigramu dla dwóch obserwacji, bo nie ma błędu w zdaniu, tzn. brakuje słowa z błędem w zdaniu.</t>
   </si>
   <si>
     <t>Cała praca</t>
@@ -260,6 +257,9 @@
   </si>
   <si>
     <t>Standardowy początek - napisać streszczenie wszystkich rozdziałów</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Przeczytać od deski do deski r. 1 oraz 6 </t>
   </si>
 </sst>
 </file>
@@ -267,10 +267,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="21">
     <font>
@@ -289,6 +289,135 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF0000FF"/>
@@ -297,141 +426,12 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="33">
     <fill>
@@ -442,6 +442,138 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -454,61 +586,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -520,36 +604,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -562,67 +616,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -633,30 +633,6 @@
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -679,7 +655,31 @@
       <right/>
       <top/>
       <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
         <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -701,15 +701,6 @@
     <border>
       <left/>
       <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
       <top style="thin">
         <color theme="4"/>
       </top>
@@ -719,17 +710,26 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
       </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
       </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
       </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -738,130 +738,130 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="6" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="26" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="11" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="14" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
@@ -870,16 +870,16 @@
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="24" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1250,7 +1250,7 @@
   <dimension ref="A1:B77"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A74" sqref="A74"/>
+      <selection activeCell="A62" sqref="$A62:$XFD62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" outlineLevelCol="1"/>
@@ -1694,9 +1694,12 @@
         <v>16</v>
       </c>
     </row>
-    <row r="60" s="1" customFormat="1" spans="1:1">
+    <row r="60" s="1" customFormat="1" hidden="1" spans="1:2">
       <c r="A60" s="1" t="s">
         <v>63</v>
+      </c>
+      <c r="B60" s="1" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="61" s="1" customFormat="1" spans="1:1">
@@ -1759,17 +1762,20 @@
         <v>75</v>
       </c>
     </row>
-    <row r="73" s="1" customFormat="1" spans="1:1">
-      <c r="A73" s="1" t="s">
+    <row r="73" spans="1:2">
+      <c r="A73" s="2" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="74" spans="1:2">
-      <c r="A74" s="2" t="s">
+      <c r="B73" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="74" hidden="1" spans="1:2">
+      <c r="A74" s="4" t="s">
         <v>77</v>
       </c>
       <c r="B74" t="s">
-        <v>3</v>
+        <v>28</v>
       </c>
     </row>
     <row r="75" hidden="1" spans="1:2">
@@ -1777,7 +1783,7 @@
         <v>78</v>
       </c>
       <c r="B75" t="s">
-        <v>28</v>
+        <v>16</v>
       </c>
     </row>
     <row r="76" spans="1:1">

</xml_diff>

<commit_message>
przed ostatnimi modyfikacjami pracy 07092019
</commit_message>
<xml_diff>
--- a/TODO_lic.xlsx
+++ b/TODO_lic.xlsx
@@ -4,20 +4,20 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowHeight="18240"/>
+    <workbookView windowWidth="27795" windowHeight="12435"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$B$81</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$B$82</definedName>
   </definedNames>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="86">
   <si>
     <t>Zadanie</t>
   </si>
@@ -40,12 +40,18 @@
     <t>Rozdział 1</t>
   </si>
   <si>
+    <t>Czym jest NLP</t>
+  </si>
+  <si>
     <t>Korekta tekstu jako proofreading oraz spellchecking</t>
   </si>
   <si>
     <t>Sukcesy noisy channel</t>
   </si>
   <si>
+    <t>done</t>
+  </si>
+  <si>
     <t>Języki, w których używano noisy channel model</t>
   </si>
   <si>
@@ -65,9 +71,6 @@
   </si>
   <si>
     <t>Zmiana kolejności według porady AW</t>
-  </si>
-  <si>
-    <t>done</t>
   </si>
   <si>
     <t>Problem przypisu z podziałem spell-checkerów</t>
@@ -279,10 +282,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="21">
     <font>
@@ -301,6 +304,89 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <i/>
       <sz val="11"/>
       <color rgb="FF7F7F7F"/>
@@ -309,6 +395,51 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
       <color rgb="FFFFFFFF"/>
@@ -316,134 +447,6 @@
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="33">
     <fill>
@@ -454,187 +457,187 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -648,17 +651,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -667,7 +664,7 @@
       <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4"/>
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -731,17 +728,23 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
       <bottom style="double">
-        <color rgb="FFFF8001"/>
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -750,148 +753,148 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="8" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="7" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="8" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="28" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1259,10 +1262,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:B81"/>
+  <dimension ref="A1:B82"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="A77" sqref="A77"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" outlineLevelCol="1"/>
@@ -1314,48 +1317,51 @@
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:1">
+    <row r="8" hidden="1" spans="1:2">
       <c r="A8" s="4" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="9" ht="28.5" spans="1:1">
+      <c r="B8" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1">
       <c r="A9" s="4" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2">
-      <c r="A10" s="2" t="s">
         <v>11</v>
       </c>
+    </row>
+    <row r="10" ht="28.5" hidden="1" spans="1:2">
+      <c r="A10" s="4" t="s">
+        <v>12</v>
+      </c>
       <c r="B10" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2">
+      <c r="A11" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B11" t="s">
         <v>3</v>
-      </c>
-    </row>
-    <row r="11" spans="1:1">
-      <c r="A11" s="4" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="12" spans="1:1">
       <c r="A12" s="4" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2">
-      <c r="A13" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B13" t="s">
+    </row>
+    <row r="13" spans="1:1">
+      <c r="A13" s="4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2">
+      <c r="A14" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B14" t="s">
         <v>3</v>
-      </c>
-    </row>
-    <row r="14" hidden="1" spans="1:2">
-      <c r="A14" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="B14" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="15" hidden="1" spans="1:2">
@@ -1363,7 +1369,7 @@
         <v>17</v>
       </c>
       <c r="B15" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
     </row>
     <row r="16" hidden="1" spans="1:2">
@@ -1371,7 +1377,7 @@
         <v>18</v>
       </c>
       <c r="B16" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
     </row>
     <row r="17" hidden="1" spans="1:2">
@@ -1379,7 +1385,7 @@
         <v>19</v>
       </c>
       <c r="B17" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
     </row>
     <row r="18" hidden="1" spans="1:2">
@@ -1387,7 +1393,7 @@
         <v>20</v>
       </c>
       <c r="B18" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
     </row>
     <row r="19" hidden="1" spans="1:2">
@@ -1395,7 +1401,7 @@
         <v>21</v>
       </c>
       <c r="B19" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
     </row>
     <row r="20" hidden="1" spans="1:2">
@@ -1403,7 +1409,7 @@
         <v>22</v>
       </c>
       <c r="B20" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
     </row>
     <row r="21" hidden="1" spans="1:2">
@@ -1411,7 +1417,7 @@
         <v>23</v>
       </c>
       <c r="B21" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
     </row>
     <row r="22" hidden="1" spans="1:2">
@@ -1419,7 +1425,7 @@
         <v>24</v>
       </c>
       <c r="B22" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
     </row>
     <row r="23" hidden="1" spans="1:2">
@@ -1427,7 +1433,7 @@
         <v>25</v>
       </c>
       <c r="B23" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
     </row>
     <row r="24" hidden="1" spans="1:2">
@@ -1435,57 +1441,63 @@
         <v>26</v>
       </c>
       <c r="B24" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
     </row>
     <row r="25" hidden="1" spans="1:2">
-      <c r="A25" s="2" t="s">
+      <c r="A25" s="4" t="s">
         <v>27</v>
       </c>
       <c r="B25" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="26" hidden="1" spans="1:2">
+      <c r="A26" s="2" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="26" ht="28.5" hidden="1" spans="1:2">
-      <c r="A26" s="4" t="s">
+      <c r="B26" t="s">
         <v>29</v>
       </c>
-      <c r="B26" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="27" hidden="1" spans="1:2">
+    </row>
+    <row r="27" ht="28.5" hidden="1" spans="1:2">
       <c r="A27" s="4" t="s">
         <v>30</v>
       </c>
       <c r="B27" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="28" spans="1:1">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="28" hidden="1" spans="1:2">
       <c r="A28" s="4" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="29" spans="1:2">
-      <c r="A29" s="2" t="s">
+      <c r="B28" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="29" hidden="1" spans="1:2">
+      <c r="A29" s="4" t="s">
         <v>32</v>
       </c>
       <c r="B29" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2">
+      <c r="A30" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B30" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="30" hidden="1" spans="1:2">
-      <c r="A30" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="B30" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="31" spans="1:1">
+    <row r="31" hidden="1" spans="1:2">
       <c r="A31" s="4" t="s">
         <v>34</v>
+      </c>
+      <c r="B31" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="32" hidden="1" spans="1:2">
@@ -1493,7 +1505,7 @@
         <v>35</v>
       </c>
       <c r="B32" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
     </row>
     <row r="33" hidden="1" spans="1:2">
@@ -1501,7 +1513,7 @@
         <v>36</v>
       </c>
       <c r="B33" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
     </row>
     <row r="34" hidden="1" spans="1:2">
@@ -1509,7 +1521,7 @@
         <v>37</v>
       </c>
       <c r="B34" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
     </row>
     <row r="35" hidden="1" spans="1:2">
@@ -1517,23 +1529,23 @@
         <v>38</v>
       </c>
       <c r="B35" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="36" ht="28.5" hidden="1" spans="1:2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="36" hidden="1" spans="1:2">
       <c r="A36" s="4" t="s">
         <v>39</v>
       </c>
       <c r="B36" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="37" hidden="1" spans="1:2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="37" ht="28.5" hidden="1" spans="1:2">
       <c r="A37" s="4" t="s">
         <v>40</v>
       </c>
       <c r="B37" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
     </row>
     <row r="38" hidden="1" spans="1:2">
@@ -1541,7 +1553,7 @@
         <v>41</v>
       </c>
       <c r="B38" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
     </row>
     <row r="39" hidden="1" spans="1:2">
@@ -1549,7 +1561,7 @@
         <v>42</v>
       </c>
       <c r="B39" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
     </row>
     <row r="40" hidden="1" spans="1:2">
@@ -1557,7 +1569,7 @@
         <v>43</v>
       </c>
       <c r="B40" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
     </row>
     <row r="41" hidden="1" spans="1:2">
@@ -1565,7 +1577,7 @@
         <v>44</v>
       </c>
       <c r="B41" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
     </row>
     <row r="42" hidden="1" spans="1:2">
@@ -1573,7 +1585,7 @@
         <v>45</v>
       </c>
       <c r="B42" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
     </row>
     <row r="43" hidden="1" spans="1:2">
@@ -1581,7 +1593,7 @@
         <v>46</v>
       </c>
       <c r="B43" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
     </row>
     <row r="44" hidden="1" spans="1:2">
@@ -1589,7 +1601,7 @@
         <v>47</v>
       </c>
       <c r="B44" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
     </row>
     <row r="45" hidden="1" spans="1:2">
@@ -1597,7 +1609,7 @@
         <v>48</v>
       </c>
       <c r="B45" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
     </row>
     <row r="46" hidden="1" spans="1:2">
@@ -1605,7 +1617,7 @@
         <v>49</v>
       </c>
       <c r="B46" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
     </row>
     <row r="47" hidden="1" spans="1:2">
@@ -1613,7 +1625,7 @@
         <v>50</v>
       </c>
       <c r="B47" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
     </row>
     <row r="48" hidden="1" spans="1:2">
@@ -1621,7 +1633,7 @@
         <v>51</v>
       </c>
       <c r="B48" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
     </row>
     <row r="49" hidden="1" spans="1:2">
@@ -1629,7 +1641,7 @@
         <v>52</v>
       </c>
       <c r="B49" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
     </row>
     <row r="50" hidden="1" spans="1:2">
@@ -1637,23 +1649,23 @@
         <v>53</v>
       </c>
       <c r="B50" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="51" ht="42.75" hidden="1" spans="1:2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="51" hidden="1" spans="1:2">
       <c r="A51" s="4" t="s">
         <v>54</v>
       </c>
       <c r="B51" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="52" hidden="1" spans="1:2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="52" ht="42.75" hidden="1" spans="1:2">
       <c r="A52" s="4" t="s">
         <v>55</v>
       </c>
       <c r="B52" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
     </row>
     <row r="53" hidden="1" spans="1:2">
@@ -1661,7 +1673,7 @@
         <v>56</v>
       </c>
       <c r="B53" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
     </row>
     <row r="54" hidden="1" spans="1:2">
@@ -1669,7 +1681,7 @@
         <v>57</v>
       </c>
       <c r="B54" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
     </row>
     <row r="55" hidden="1" spans="1:2">
@@ -1677,15 +1689,15 @@
         <v>58</v>
       </c>
       <c r="B55" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="56" s="1" customFormat="1" hidden="1" spans="1:2">
-      <c r="A56" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="56" hidden="1" spans="1:2">
+      <c r="A56" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="B56" s="1" t="s">
-        <v>16</v>
+      <c r="B56" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="57" s="1" customFormat="1" hidden="1" spans="1:2">
@@ -1693,7 +1705,7 @@
         <v>60</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
     </row>
     <row r="58" s="1" customFormat="1" hidden="1" spans="1:2">
@@ -1701,7 +1713,7 @@
         <v>61</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
     </row>
     <row r="59" s="1" customFormat="1" hidden="1" spans="1:2">
@@ -1709,7 +1721,7 @@
         <v>62</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
     </row>
     <row r="60" s="1" customFormat="1" hidden="1" spans="1:2">
@@ -1717,7 +1729,7 @@
         <v>63</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>28</v>
+        <v>10</v>
       </c>
     </row>
     <row r="61" s="1" customFormat="1" hidden="1" spans="1:2">
@@ -1725,7 +1737,7 @@
         <v>64</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>16</v>
+        <v>29</v>
       </c>
     </row>
     <row r="62" s="1" customFormat="1" hidden="1" spans="1:2">
@@ -1733,7 +1745,7 @@
         <v>65</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
     </row>
     <row r="63" s="1" customFormat="1" hidden="1" spans="1:2">
@@ -1741,7 +1753,7 @@
         <v>66</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
     </row>
     <row r="64" s="1" customFormat="1" hidden="1" spans="1:2">
@@ -1749,7 +1761,7 @@
         <v>67</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
     </row>
     <row r="65" s="1" customFormat="1" hidden="1" spans="1:2">
@@ -1757,7 +1769,7 @@
         <v>68</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
     </row>
     <row r="66" s="1" customFormat="1" hidden="1" spans="1:2">
@@ -1765,7 +1777,7 @@
         <v>69</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
     </row>
     <row r="67" s="1" customFormat="1" hidden="1" spans="1:2">
@@ -1773,7 +1785,7 @@
         <v>70</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
     </row>
     <row r="68" s="1" customFormat="1" hidden="1" spans="1:2">
@@ -1781,7 +1793,7 @@
         <v>71</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
     </row>
     <row r="69" s="1" customFormat="1" hidden="1" spans="1:2">
@@ -1789,7 +1801,7 @@
         <v>72</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
     </row>
     <row r="70" s="1" customFormat="1" hidden="1" spans="1:2">
@@ -1797,7 +1809,7 @@
         <v>73</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
     </row>
     <row r="71" s="1" customFormat="1" hidden="1" spans="1:2">
@@ -1805,7 +1817,7 @@
         <v>74</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
     </row>
     <row r="72" s="1" customFormat="1" hidden="1" spans="1:2">
@@ -1813,12 +1825,15 @@
         <v>75</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="73" s="1" customFormat="1" spans="1:1">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="73" s="1" customFormat="1" hidden="1" spans="1:2">
       <c r="A73" s="1" t="s">
         <v>76</v>
+      </c>
+      <c r="B73" s="1" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="74" s="1" customFormat="1" spans="1:1">
@@ -1831,25 +1846,28 @@
         <v>78</v>
       </c>
     </row>
-    <row r="76" s="1" customFormat="1" spans="1:1">
+    <row r="76" s="1" customFormat="1" hidden="1" spans="1:2">
       <c r="A76" s="1" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="77" spans="1:2">
-      <c r="A77" s="2" t="s">
+      <c r="B76" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="77" s="1" customFormat="1" hidden="1" spans="1:2">
+      <c r="A77" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="B77" t="s">
+      <c r="B77" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2">
+      <c r="A78" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="B78" t="s">
         <v>3</v>
-      </c>
-    </row>
-    <row r="78" hidden="1" spans="1:2">
-      <c r="A78" s="4" t="s">
-        <v>81</v>
-      </c>
-      <c r="B78" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="79" hidden="1" spans="1:2">
@@ -1857,12 +1875,15 @@
         <v>82</v>
       </c>
       <c r="B79" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="80" spans="1:1">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="80" hidden="1" spans="1:2">
       <c r="A80" s="4" t="s">
         <v>83</v>
+      </c>
+      <c r="B80" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="81" spans="1:1">
@@ -1870,8 +1891,13 @@
         <v>84</v>
       </c>
     </row>
+    <row r="82" spans="1:1">
+      <c r="A82" s="4" t="s">
+        <v>85</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:B81">
+  <autoFilter ref="A1:B82">
     <filterColumn colId="1">
       <customFilters>
         <customFilter operator="equal" val=""/>

</xml_diff>

<commit_message>
commit po mailu o gotowej pracy
</commit_message>
<xml_diff>
--- a/TODO_lic.xlsx
+++ b/TODO_lic.xlsx
@@ -10,14 +10,14 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$B$122</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$B$126</definedName>
   </definedNames>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="237" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="129">
   <si>
     <t>R</t>
   </si>
@@ -43,6 +43,9 @@
     <t>Zmienić nieAPA cytowania na APA</t>
   </si>
   <si>
+    <t>Usunąć błędy związane z U301 i U328</t>
+  </si>
+  <si>
     <t>Rozdział 1</t>
   </si>
   <si>
@@ -370,7 +373,16 @@
     <t>Dodać abstrakt</t>
   </si>
   <si>
-    <t>Opracować pierwszą stronę zgodne ze wzorem kogni.</t>
+    <t>Usunąć klasyfikację tematyczną</t>
+  </si>
+  <si>
+    <t>Dodać tytuł po angielsku</t>
+  </si>
+  <si>
+    <t>Dodać słowa kluczowe po angielsku</t>
+  </si>
+  <si>
+    <t>Dodać streszczenie po angielsku</t>
   </si>
   <si>
     <t>Rozdział 2: ostateczne czytanie</t>
@@ -399,10 +411,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
   </numFmts>
   <fonts count="21">
     <font>
@@ -421,10 +433,11 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="0"/>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
       <name val="Calibri"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -443,14 +456,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
       <name val="Calibri"/>
@@ -458,17 +463,16 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
       <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -483,15 +487,37 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
+      <i/>
       <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -506,23 +532,8 @@
     </font>
     <font>
       <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -536,10 +547,10 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <sz val="18"/>
+      <color theme="3"/>
       <name val="Calibri"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -550,18 +561,19 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <sz val="15"/>
+      <color theme="3"/>
       <name val="Calibri"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -574,13 +586,85 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -592,13 +676,67 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -610,151 +748,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -765,6 +777,56 @@
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -786,43 +848,8 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
       <bottom style="double">
-        <color theme="4"/>
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -845,23 +872,8 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -870,148 +882,148 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="11" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="11" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="12" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="27" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="12" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="25" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="20" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1382,10 +1394,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:B122"/>
+  <dimension ref="A1:B126"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="B123" sqref="B123"/>
+      <selection activeCell="A128" sqref="A128"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" outlineLevelCol="1"/>
@@ -1433,20 +1445,20 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:2">
-      <c r="A6" s="2" t="s">
+    <row r="6" hidden="1" spans="1:2">
+      <c r="A6" s="5" t="s">
         <v>8</v>
       </c>
       <c r="B6" s="4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7" s="4" t="s">
         <v>3</v>
-      </c>
-    </row>
-    <row r="7" hidden="1" spans="1:2">
-      <c r="A7" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="8" hidden="1" spans="1:2">
@@ -1461,7 +1473,7 @@
       <c r="A9" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="4" t="s">
         <v>5</v>
       </c>
     </row>
@@ -1469,7 +1481,7 @@
       <c r="A10" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="B10" s="4" t="s">
+      <c r="B10" t="s">
         <v>5</v>
       </c>
     </row>
@@ -1481,15 +1493,15 @@
         <v>5</v>
       </c>
     </row>
-    <row r="12" ht="28.5" hidden="1" spans="1:2">
+    <row r="12" hidden="1" spans="1:2">
       <c r="A12" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="B12" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="13" hidden="1" spans="1:2">
+      <c r="B12" s="4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="13" ht="28.5" hidden="1" spans="1:2">
       <c r="A13" s="5" t="s">
         <v>15</v>
       </c>
@@ -1497,58 +1509,68 @@
         <v>5</v>
       </c>
     </row>
-    <row r="14" spans="1:2">
-      <c r="A14" s="2" t="s">
+    <row r="14" hidden="1" spans="1:2">
+      <c r="A14" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="B14" s="4" t="s">
+      <c r="B14" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2">
+      <c r="A15" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B15" s="4" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="15" ht="28.5" spans="1:2">
-      <c r="A15" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="B15" s="4"/>
-    </row>
-    <row r="16" spans="1:2">
+    <row r="16" ht="28.5" hidden="1" spans="1:2">
       <c r="A16" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="B16" s="4"/>
-    </row>
-    <row r="17" spans="1:2">
+      <c r="B16" s="4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="17" hidden="1" spans="1:2">
       <c r="A17" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="B17" s="4"/>
-    </row>
-    <row r="18" spans="1:2">
+      <c r="B17" s="4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="18" hidden="1" spans="1:2">
       <c r="A18" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="B18" s="4"/>
-    </row>
-    <row r="19" spans="1:2">
+      <c r="B18" s="4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="19" hidden="1" spans="1:2">
       <c r="A19" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="B19" s="4"/>
-    </row>
-    <row r="20" spans="1:2">
-      <c r="A20" s="2" t="s">
+      <c r="B19" s="4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="20" hidden="1" spans="1:2">
+      <c r="A20" s="5" t="s">
         <v>22</v>
       </c>
       <c r="B20" s="4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2">
+      <c r="A21" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B21" s="4" t="s">
         <v>3</v>
-      </c>
-    </row>
-    <row r="21" hidden="1" spans="1:2">
-      <c r="A21" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="B21" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="22" hidden="1" spans="1:2">
@@ -1632,27 +1654,27 @@
       </c>
     </row>
     <row r="32" hidden="1" spans="1:2">
-      <c r="A32" s="2" t="s">
+      <c r="A32" s="5" t="s">
         <v>34</v>
       </c>
       <c r="B32" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="33" hidden="1" spans="1:2">
+      <c r="A33" s="2" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="33" ht="28.5" hidden="1" spans="1:2">
-      <c r="A33" s="5" t="s">
+      <c r="B33" t="s">
         <v>36</v>
       </c>
-      <c r="B33" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="34" hidden="1" spans="1:2">
+    </row>
+    <row r="34" ht="28.5" hidden="1" spans="1:2">
       <c r="A34" s="5" t="s">
         <v>37</v>
       </c>
       <c r="B34" t="s">
-        <v>5</v>
+        <v>36</v>
       </c>
     </row>
     <row r="35" hidden="1" spans="1:2">
@@ -1713,7 +1735,7 @@
     </row>
     <row r="42" hidden="1" spans="1:2">
       <c r="A42" s="5" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B42" t="s">
         <v>5</v>
@@ -1723,24 +1745,24 @@
       <c r="A43" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="B43" s="4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="44" spans="1:2">
-      <c r="A44" s="2" t="s">
+      <c r="B43" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="44" hidden="1" spans="1:2">
+      <c r="A44" s="5" t="s">
         <v>46</v>
       </c>
       <c r="B44" s="4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2">
+      <c r="A45" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="B45" s="4" t="s">
         <v>3</v>
-      </c>
-    </row>
-    <row r="45" hidden="1" spans="1:2">
-      <c r="A45" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="B45" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="46" hidden="1" spans="1:2">
@@ -1783,7 +1805,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="51" ht="28.5" hidden="1" spans="1:2">
+    <row r="51" hidden="1" spans="1:2">
       <c r="A51" s="5" t="s">
         <v>53</v>
       </c>
@@ -1791,7 +1813,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="52" hidden="1" spans="1:2">
+    <row r="52" ht="28.5" hidden="1" spans="1:2">
       <c r="A52" s="5" t="s">
         <v>54</v>
       </c>
@@ -1903,7 +1925,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="66" ht="42.75" hidden="1" spans="1:2">
+    <row r="66" hidden="1" spans="1:2">
       <c r="A66" s="5" t="s">
         <v>68</v>
       </c>
@@ -1911,7 +1933,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="67" hidden="1" spans="1:2">
+    <row r="67" ht="42.75" hidden="1" spans="1:2">
       <c r="A67" s="5" t="s">
         <v>69</v>
       </c>
@@ -1943,11 +1965,11 @@
         <v>5</v>
       </c>
     </row>
-    <row r="71" s="1" customFormat="1" hidden="1" spans="1:2">
-      <c r="A71" s="1" t="s">
+    <row r="71" hidden="1" spans="1:2">
+      <c r="A71" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="B71" s="1" t="s">
+      <c r="B71" t="s">
         <v>5</v>
       </c>
     </row>
@@ -1980,7 +2002,7 @@
         <v>77</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>35</v>
+        <v>5</v>
       </c>
     </row>
     <row r="76" s="1" customFormat="1" hidden="1" spans="1:2">
@@ -1988,7 +2010,7 @@
         <v>78</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>5</v>
+        <v>36</v>
       </c>
     </row>
     <row r="77" s="1" customFormat="1" hidden="1" spans="1:2">
@@ -2163,7 +2185,7 @@
       <c r="A98" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="B98" s="4" t="s">
+      <c r="B98" s="1" t="s">
         <v>5</v>
       </c>
     </row>
@@ -2179,7 +2201,7 @@
       <c r="A100" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="B100" s="1" t="s">
+      <c r="B100" s="4" t="s">
         <v>5</v>
       </c>
     </row>
@@ -2239,36 +2261,36 @@
         <v>5</v>
       </c>
     </row>
-    <row r="108" s="1" customFormat="1" spans="1:2">
-      <c r="A108" s="4" t="s">
+    <row r="108" s="1" customFormat="1" hidden="1" spans="1:2">
+      <c r="A108" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="B108" s="4" t="s">
+      <c r="B108" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="109" s="1" customFormat="1" spans="1:2">
+      <c r="A109" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="B109" s="4" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="109" s="1" customFormat="1" hidden="1" spans="1:2">
-      <c r="A109" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="B109" s="4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="110" spans="1:2">
-      <c r="A110" s="2" t="s">
+    <row r="110" s="1" customFormat="1" hidden="1" spans="1:2">
+      <c r="A110" s="1" t="s">
         <v>112</v>
       </c>
       <c r="B110" s="4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="111" spans="1:2">
+      <c r="A111" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="B111" s="4" t="s">
         <v>3</v>
-      </c>
-    </row>
-    <row r="111" hidden="1" spans="1:2">
-      <c r="A111" s="5" t="s">
-        <v>113</v>
-      </c>
-      <c r="B111" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="112" hidden="1" spans="1:2">
@@ -2276,12 +2298,15 @@
         <v>114</v>
       </c>
       <c r="B112" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="113" spans="1:1">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="113" hidden="1" spans="1:2">
       <c r="A113" s="5" t="s">
         <v>115</v>
+      </c>
+      <c r="B113" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="114" hidden="1" spans="1:2">
@@ -2292,9 +2317,12 @@
         <v>5</v>
       </c>
     </row>
-    <row r="115" spans="1:1">
+    <row r="115" hidden="1" spans="1:2">
       <c r="A115" s="5" t="s">
         <v>117</v>
+      </c>
+      <c r="B115" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="116" hidden="1" spans="1:2">
@@ -2353,11 +2381,42 @@
         <v>5</v>
       </c>
     </row>
+    <row r="123" hidden="1" spans="1:2">
+      <c r="A123" s="5" t="s">
+        <v>125</v>
+      </c>
+      <c r="B123" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="124" hidden="1" spans="1:2">
+      <c r="A124" s="5" t="s">
+        <v>126</v>
+      </c>
+      <c r="B124" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="125" hidden="1" spans="1:2">
+      <c r="A125" s="5" t="s">
+        <v>127</v>
+      </c>
+      <c r="B125" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="126" hidden="1" spans="1:2">
+      <c r="A126" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="B126" t="s">
+        <v>5</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:B122">
+  <autoFilter ref="A1:B126">
     <filterColumn colId="1">
       <customFilters>
-        <customFilter operator="equal" val=""/>
         <customFilter operator="equal" val="sec"/>
       </customFilters>
     </filterColumn>

</xml_diff>

<commit_message>
nowe zadania do excela
</commit_message>
<xml_diff>
--- a/TODO_lic.xlsx
+++ b/TODO_lic.xlsx
@@ -10,14 +10,14 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$B$126</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$B$136</definedName>
   </definedNames>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="262" uniqueCount="139">
   <si>
     <t>R</t>
   </si>
@@ -352,6 +352,30 @@
     <t>Rozmieszczenie tabelek w omówieniu wyników</t>
   </si>
   <si>
+    <t>obrazek - opis i przypis</t>
+  </si>
+  <si>
+    <t>problem uzgodnienia</t>
+  </si>
+  <si>
+    <t>odwołanie do dalszej części pracy - usunąć</t>
+  </si>
+  <si>
+    <t>przenieść na poprzednią stronę.</t>
+  </si>
+  <si>
+    <t>usunąć fragment baseline</t>
+  </si>
+  <si>
+    <t>odniesienie bibliograficzne</t>
+  </si>
+  <si>
+    <t>przenieść fragment podsumowania</t>
+  </si>
+  <si>
+    <t>macierz pod rozdziałem 6.3</t>
+  </si>
+  <si>
     <t>Kod</t>
   </si>
   <si>
@@ -401,6 +425,12 @@
   </si>
   <si>
     <t>Rozdział 6: ostateczne czytanie</t>
+  </si>
+  <si>
+    <t>Napisać w mailu do AW, że trudno się umieszcza tabele dokładnie w miejscach, gdzie chcemy. Miałem z tym wcześniej problemy.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> zdanie we wstępie, co jest celem pracy (to może być parafraza tytułu) i odnieść się do tego w podsumowaniu, tzn. że cel został osiągnięty.</t>
   </si>
   <si>
     <t xml:space="preserve">Przeczytać od deski do deski r. 1 oraz 6 </t>
@@ -433,6 +463,14 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="13"/>
       <color theme="3"/>
@@ -442,7 +480,60 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -457,45 +548,14 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -510,13 +570,6 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
@@ -525,7 +578,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -540,42 +593,19 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
+      <i/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="33">
     <fill>
@@ -586,25 +616,145 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
+        <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -616,55 +766,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -676,97 +778,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -789,6 +819,15 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FF7F7F7F"/>
       </left>
@@ -800,17 +839,6 @@
       </top>
       <bottom style="thin">
         <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -830,26 +858,22 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left/>
       <right/>
-      <top/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
       <bottom style="double">
-        <color rgb="FFFF8001"/>
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -869,11 +893,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -882,148 +912,148 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="11" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="16" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="11" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="28" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="6" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="25" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="17" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1394,10 +1424,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:B126"/>
+  <dimension ref="A1:B136"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="A128" sqref="A128"/>
+      <selection activeCell="A109" sqref="A109"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" outlineLevelCol="1"/>
@@ -2269,92 +2299,68 @@
         <v>5</v>
       </c>
     </row>
-    <row r="109" s="1" customFormat="1" spans="1:2">
-      <c r="A109" s="4" t="s">
+    <row r="109" s="1" customFormat="1" spans="1:1">
+      <c r="A109" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="B109" s="4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="110" s="1" customFormat="1" hidden="1" spans="1:2">
+    </row>
+    <row r="110" s="1" customFormat="1" spans="1:1">
       <c r="A110" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="B110" s="4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="111" spans="1:2">
-      <c r="A111" s="2" t="s">
+    </row>
+    <row r="111" s="1" customFormat="1" spans="1:1">
+      <c r="A111" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="B111" s="4" t="s">
+    </row>
+    <row r="112" s="1" customFormat="1" spans="1:1">
+      <c r="A112" s="1" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="113" s="1" customFormat="1" spans="1:1">
+      <c r="A113" s="1" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="114" s="1" customFormat="1" spans="1:1">
+      <c r="A114" s="1" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="115" s="1" customFormat="1" spans="1:1">
+      <c r="A115" s="1" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="116" s="1" customFormat="1" spans="1:1">
+      <c r="A116" s="1" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="117" s="1" customFormat="1" spans="1:2">
+      <c r="A117" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="B117" s="4" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="112" hidden="1" spans="1:2">
-      <c r="A112" s="5" t="s">
-        <v>114</v>
-      </c>
-      <c r="B112" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="113" hidden="1" spans="1:2">
-      <c r="A113" s="5" t="s">
-        <v>115</v>
-      </c>
-      <c r="B113" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="114" hidden="1" spans="1:2">
-      <c r="A114" s="5" t="s">
-        <v>116</v>
-      </c>
-      <c r="B114" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="115" hidden="1" spans="1:2">
-      <c r="A115" s="5" t="s">
-        <v>117</v>
-      </c>
-      <c r="B115" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="116" hidden="1" spans="1:2">
-      <c r="A116" s="5" t="s">
-        <v>118</v>
-      </c>
-      <c r="B116" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="117" hidden="1" spans="1:2">
-      <c r="A117" s="5" t="s">
-        <v>119</v>
-      </c>
-      <c r="B117" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="118" hidden="1" spans="1:2">
-      <c r="A118" s="5" t="s">
+    <row r="118" s="1" customFormat="1" hidden="1" spans="1:2">
+      <c r="A118" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="B118" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="119" hidden="1" spans="1:2">
-      <c r="A119" s="5" t="s">
+      <c r="B118" s="4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="119" spans="1:2">
+      <c r="A119" s="2" t="s">
         <v>121</v>
       </c>
-      <c r="B119" t="s">
-        <v>5</v>
+      <c r="B119" s="4" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="120" hidden="1" spans="1:2">
@@ -2362,7 +2368,7 @@
         <v>122</v>
       </c>
       <c r="B120" t="s">
-        <v>5</v>
+        <v>36</v>
       </c>
     </row>
     <row r="121" hidden="1" spans="1:2">
@@ -2413,10 +2419,85 @@
         <v>5</v>
       </c>
     </row>
+    <row r="127" hidden="1" spans="1:2">
+      <c r="A127" s="5" t="s">
+        <v>129</v>
+      </c>
+      <c r="B127" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="128" hidden="1" spans="1:2">
+      <c r="A128" s="5" t="s">
+        <v>130</v>
+      </c>
+      <c r="B128" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="129" hidden="1" spans="1:2">
+      <c r="A129" s="5" t="s">
+        <v>131</v>
+      </c>
+      <c r="B129" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="130" hidden="1" spans="1:2">
+      <c r="A130" s="5" t="s">
+        <v>132</v>
+      </c>
+      <c r="B130" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="131" hidden="1" spans="1:2">
+      <c r="A131" s="5" t="s">
+        <v>133</v>
+      </c>
+      <c r="B131" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="132" hidden="1" spans="1:2">
+      <c r="A132" s="5" t="s">
+        <v>134</v>
+      </c>
+      <c r="B132" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="133" hidden="1" spans="1:2">
+      <c r="A133" s="5" t="s">
+        <v>135</v>
+      </c>
+      <c r="B133" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="134" spans="1:1">
+      <c r="A134" s="5" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="135" spans="1:1">
+      <c r="A135" s="5" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="136" hidden="1" spans="1:2">
+      <c r="A136" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="B136" t="s">
+        <v>5</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:B126">
+  <autoFilter ref="A1:B136">
     <filterColumn colId="1">
       <customFilters>
+        <customFilter operator="equal" val=""/>
         <customFilter operator="equal" val="sec"/>
       </customFilters>
     </filterColumn>

</xml_diff>